<commit_message>
Completed test cases 10,11,15-19,21
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/WorkbookUtilitiesModuleTest.xlsx
+++ b/resources/ExcelsheetData/WorkbookUtilitiesModuleTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="TC_WU_001" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,12 @@
     <sheet name="TC_WU_004" sheetId="3" r:id="rId4"/>
     <sheet name="TC_WU_006" sheetId="4" r:id="rId5"/>
     <sheet name="TC_WU_007" sheetId="5" r:id="rId6"/>
-    <sheet name="TC_PRODUCTS_007" sheetId="6" r:id="rId7"/>
-    <sheet name="TC_PRODUCTS_008" sheetId="7" r:id="rId8"/>
-    <sheet name="TC_PRODUCTS_009" sheetId="8" r:id="rId9"/>
-    <sheet name="TC_PRODUCTS_010" sheetId="9" r:id="rId10"/>
-    <sheet name="TC_PRODUCTS_011" sheetId="13" r:id="rId11"/>
-    <sheet name="TC_PRODUCTS_013" sheetId="14" r:id="rId12"/>
+    <sheet name="TC_WU_013_14" sheetId="6" r:id="rId7"/>
+    <sheet name="TC_WU_015" sheetId="7" r:id="rId8"/>
+    <sheet name="TC_WU_016" sheetId="8" r:id="rId9"/>
+    <sheet name="TC_WU_017" sheetId="9" r:id="rId10"/>
+    <sheet name="TC_WU_018" sheetId="13" r:id="rId11"/>
+    <sheet name="TC_WU_019" sheetId="14" r:id="rId12"/>
     <sheet name="TC_PRODUCTS_015" sheetId="11" r:id="rId13"/>
     <sheet name="TC_PRODUCTS_018" sheetId="15" r:id="rId14"/>
     <sheet name="TC_PRODUCTS_020" sheetId="16" r:id="rId15"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t>Product Removal Success Message</t>
   </si>
@@ -36,105 +36,6 @@
     <t>Product deleted successfully</t>
   </si>
   <si>
-    <r>
-      <t>Product Images Fields</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Asterisk has to be inculded for mandatory fields)</t>
-    </r>
-  </si>
-  <si>
-    <t>Action, Image, Image Name</t>
-  </si>
-  <si>
-    <t>Image Desc, Product Image URL, Upload Product Image</t>
-  </si>
-  <si>
-    <r>
-      <t>Add New Product Images Fields</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Asterisk has to be inculded for mandatory fields)</t>
-    </r>
-  </si>
-  <si>
-    <t>Product Image Description</t>
-  </si>
-  <si>
-    <t>Product Image URL</t>
-  </si>
-  <si>
-    <t>Product Image success Message</t>
-  </si>
-  <si>
-    <t>Product Image URL saved Successfully</t>
-  </si>
-  <si>
-    <t>http://imaging.nikon.com/lineup/lens/zoom/normalzoom/af-s_dx_18-300mmf_35-56g_ed_vr/img/sample/sample1_l.jpg</t>
-  </si>
-  <si>
-    <t>AutomationTest Image</t>
-  </si>
-  <si>
-    <t>Product Image Upload Success Message</t>
-  </si>
-  <si>
-    <t>Product Image saved Successfully</t>
-  </si>
-  <si>
-    <t>Product Image File location</t>
-  </si>
-  <si>
-    <t>C:\Users\rameshwar.j\Pictures\Screenshots\Screenshot.png</t>
-  </si>
-  <si>
-    <t>Product Image Remove Success Message</t>
-  </si>
-  <si>
-    <t>1 Image removed Successfully</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Item assigned to product message
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Note: Do not include the product name in the success message</t>
-    </r>
-  </si>
-  <si>
-    <t>Assigned Items Saved Successfully to Product</t>
-  </si>
-  <si>
     <t>General Info,Descriptions,Products,Keywords,Documents,Images,Videos,Linked Items,Attributes,Custom Prices, Categorization,Custom Fields,Warehouse,Customer PartNumber,User Review</t>
   </si>
   <si>
@@ -193,13 +94,61 @@
   </si>
   <si>
     <t>Action,Item Id,Item Image, Part Number,Manufacturer Part Number,Item Status,Display Online,Quantity Available,List Price,Short Description</t>
+  </si>
+  <si>
+    <t>PrtNum</t>
+  </si>
+  <si>
+    <t>Excel sheet name (Sheet name in WorkbookItemsTemplate.xlsx)</t>
+  </si>
+  <si>
+    <t>Item(s) added to Workbook.</t>
+  </si>
+  <si>
+    <t>Items added success message (DON'T INCLUDE THE NUMBER OF ITEM)</t>
+  </si>
+  <si>
+    <t>Excel Sheet Path</t>
+  </si>
+  <si>
+    <t>resources/ExcelsheetData/WorkbookUploadTemplates/WorkbookItemsTemplate-PN.xlsx</t>
+  </si>
+  <si>
+    <t>Prt_Mname</t>
+  </si>
+  <si>
+    <t>resources/ExcelsheetData/WorkbookUploadTemplates/WorkbookItemsTemplate-PN-MN.xlsx</t>
+  </si>
+  <si>
+    <t>Prt_Brnd_Mname</t>
+  </si>
+  <si>
+    <t>resources/ExcelsheetData/WorkbookUploadTemplates/WorkbookItemsTemplate-PN-BN-MN.xlsx</t>
+  </si>
+  <si>
+    <t>Mprt_Mname</t>
+  </si>
+  <si>
+    <t>resources/ExcelsheetData/WorkbookUploadTemplates/WorkbookItemsTemplate-MPN-MN.xlsx</t>
+  </si>
+  <si>
+    <t>Mprt_Brnd</t>
+  </si>
+  <si>
+    <t>resources/ExcelsheetData/WorkbookUploadTemplates/WorkbookItemsTemplate-MPN-BN.xlsx</t>
+  </si>
+  <si>
+    <t>resources/ExcelsheetData/WorkbookUploadTemplates/WorkbookItemsTemplate-UPC.xlsx</t>
+  </si>
+  <si>
+    <t>Upc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,34 +175,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF008000"/>
-      <name val="Trebuchet MS"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF008000"/>
-      <name val="Trebuchet MS"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -294,27 +215,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -325,8 +236,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -640,47 +550,54 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75">
-      <c r="A2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>13</v>
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="45">
+      <c r="A2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -691,25 +608,39 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="36.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="16.5">
-      <c r="A2" s="7" t="s">
-        <v>17</v>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="45">
+      <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -719,25 +650,39 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="45">
-      <c r="A1" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="3" t="s">
-        <v>19</v>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="45">
+      <c r="A2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -788,12 +733,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="60">
-      <c r="A2" s="9" t="s">
-        <v>20</v>
+      <c r="A2" s="5" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -817,18 +762,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>24</v>
+      <c r="A2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -851,12 +796,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -880,25 +825,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>34</v>
+      <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -921,13 +866,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="5" t="s">
-        <v>36</v>
+      <c r="A1" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="11" t="s">
-        <v>37</v>
+      <c r="A2" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -948,19 +893,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="50.25" customHeight="1">
-      <c r="A1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>32</v>
+      <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -972,7 +917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -983,12 +928,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -998,51 +943,82 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="51.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="45">
       <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="65.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="45">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1055,42 +1031,39 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="39" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="45">
       <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
+        <v>31</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completed test scripts 22-26
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/WorkbookUtilitiesModuleTest.xlsx
+++ b/resources/ExcelsheetData/WorkbookUtilitiesModuleTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="11"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="TC_WU_001" sheetId="1" r:id="rId1"/>
@@ -19,40 +19,17 @@
     <sheet name="TC_WU_017" sheetId="9" r:id="rId10"/>
     <sheet name="TC_WU_018" sheetId="13" r:id="rId11"/>
     <sheet name="TC_WU_019" sheetId="14" r:id="rId12"/>
-    <sheet name="TC_PRODUCTS_015" sheetId="11" r:id="rId13"/>
-    <sheet name="TC_PRODUCTS_018" sheetId="15" r:id="rId14"/>
-    <sheet name="TC_PRODUCTS_020" sheetId="16" r:id="rId15"/>
+    <sheet name="TC_WU_022" sheetId="11" r:id="rId13"/>
+    <sheet name="TC_WU_023" sheetId="15" r:id="rId14"/>
+    <sheet name="TC_WU_024" sheetId="16" r:id="rId15"/>
+    <sheet name="TC_WU_026" sheetId="17" r:id="rId16"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
-  <si>
-    <t>Product Removal Success Message</t>
-  </si>
-  <si>
-    <t>Product deleted successfully</t>
-  </si>
-  <si>
-    <t>General Info,Descriptions,Products,Keywords,Documents,Images,Videos,Linked Items,Attributes,Custom Prices, Categorization,Custom Fields,Warehouse,Customer PartNumber,User Review</t>
-  </si>
-  <si>
-    <t>Edit Item Fields</t>
-  </si>
-  <si>
-    <t>Item Part Number</t>
-  </si>
-  <si>
-    <t>Number of Copies</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>AutomationTestItem 3313</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
   <si>
     <t>WorkBook,Import Items to Workbook, Bulk Item Categorization, Items To Subset, Items To New Brand</t>
   </si>
@@ -142,13 +119,60 @@
   </si>
   <si>
     <t>Upc</t>
+  </si>
+  <si>
+    <t>Bulk Item Categorization Success Message</t>
+  </si>
+  <si>
+    <t>Item(s) is/are assigned to Category Successfully.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Items added success message </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(DON'T INCLUDE THE NUMBER OF ITEMS)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Bulk Item Categorization Success Message </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(DON'T INCLUDE THE NUMBER OF ITEMS)</t>
+    </r>
+  </si>
+  <si>
+    <t>All Items are successfully removed from the Category.</t>
+  </si>
+  <si>
+    <t>Items To Subset Success Message</t>
+  </si>
+  <si>
+    <t>Item(s) is/are added to Subset Successfully.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +196,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF008000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -218,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -226,12 +258,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -550,12 +576,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -580,24 +606,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="45">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -623,24 +649,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="45">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -652,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -665,28 +691,29 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="45">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -700,17 +727,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="76.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -733,75 +760,96 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="60">
-      <c r="A2" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="49.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="49.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="93.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
         <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="33.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="93.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -826,24 +874,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -867,12 +915,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="4" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="7" t="s">
-        <v>19</v>
+      <c r="A2" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -894,18 +942,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="50.25" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -928,12 +976,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -958,24 +1006,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="45">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1001,24 +1049,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="45">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1043,24 +1091,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="45">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added AutoIt support for file Upload
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/WorkbookUtilitiesModuleTest.xlsx
+++ b/resources/ExcelsheetData/WorkbookUtilitiesModuleTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="8" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="TC_WU_001" sheetId="1" r:id="rId1"/>
@@ -13,18 +13,18 @@
     <sheet name="TC_WU_004" sheetId="3" r:id="rId4"/>
     <sheet name="TC_WU_006" sheetId="4" r:id="rId5"/>
     <sheet name="TC_WU_007" sheetId="5" r:id="rId6"/>
-    <sheet name="TC_WU_009" sheetId="20" r:id="rId7"/>
-    <sheet name="TC_WU_013_14" sheetId="6" r:id="rId8"/>
-    <sheet name="TC_WU_015" sheetId="7" r:id="rId9"/>
-    <sheet name="TC_WU_016" sheetId="8" r:id="rId10"/>
-    <sheet name="TC_WU_017" sheetId="9" r:id="rId11"/>
-    <sheet name="TC_WU_018" sheetId="13" r:id="rId12"/>
-    <sheet name="TC_WU_019" sheetId="14" r:id="rId13"/>
-    <sheet name="TC_WU_022" sheetId="11" r:id="rId14"/>
-    <sheet name="TC_WU_023" sheetId="15" r:id="rId15"/>
-    <sheet name="TC_WU_024" sheetId="16" r:id="rId16"/>
-    <sheet name="TC_WU_026" sheetId="17" r:id="rId17"/>
-    <sheet name="TC_WU_027" sheetId="18" r:id="rId18"/>
+    <sheet name="TC_WU_008" sheetId="21" r:id="rId7"/>
+    <sheet name="TC_WU_009" sheetId="20" r:id="rId8"/>
+    <sheet name="TC_WU_013_14" sheetId="6" r:id="rId9"/>
+    <sheet name="TC_WU_015" sheetId="7" r:id="rId10"/>
+    <sheet name="TC_WU_016" sheetId="8" r:id="rId11"/>
+    <sheet name="TC_WU_017" sheetId="9" r:id="rId12"/>
+    <sheet name="TC_WU_018" sheetId="13" r:id="rId13"/>
+    <sheet name="TC_WU_019" sheetId="14" r:id="rId14"/>
+    <sheet name="TC_WU_022" sheetId="11" r:id="rId15"/>
+    <sheet name="TC_WU_023" sheetId="15" r:id="rId16"/>
+    <sheet name="TC_WU_024" sheetId="16" r:id="rId17"/>
+    <sheet name="TC_WU_026_27" sheetId="17" r:id="rId18"/>
     <sheet name="TC_WU_028" sheetId="19" r:id="rId19"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
   <si>
     <t>WorkBook,Import Items to Workbook, Bulk Item Categorization, Items To Subset, Items To New Brand</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>Updated Workbook Name</t>
-  </si>
-  <si>
-    <t>AutomationTestWorkBook Updated 1</t>
   </si>
   <si>
     <t>Save Blank work error message</t>
@@ -171,9 +168,6 @@
     <t>Item(s) is/are removed from Subset Successfully.</t>
   </si>
   <si>
-    <t>Workbook Items assigned to New Brand Successfully</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Items To Subset Success Message </t>
     </r>
@@ -239,6 +233,28 @@
       </rPr>
       <t>(DON'T INCLUDE THE NUMBER OF ITEMS)</t>
     </r>
+  </si>
+  <si>
+    <t>AutomationTestWorkBook Updated 1</t>
+  </si>
+  <si>
+    <r>
+      <t>Remove single item Success Message</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (DON'T INCLUDE THE NUMBER OF ITEMS)</t>
+    </r>
+  </si>
+  <si>
+    <t>Workbook Items assigned to New Brand Successfully.</t>
   </si>
 </sst>
 </file>
@@ -349,6 +365,51 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="storeItemListTableFormId:j_id972" descr="https://template.cimm2.com/CIMM2Touch/a4j/g/3_3_3.Finalimages/spacer.gif.jsf"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="190500"/>
+          <a:ext cx="9525" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -667,7 +728,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="A2" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -679,24 +740,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="45">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -709,7 +770,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -721,29 +782,28 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="45">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -752,7 +812,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -764,13 +824,98 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="45">
+      <c r="A2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="45">
+      <c r="A2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="45">
@@ -778,23 +923,381 @@
         <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="76.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="71.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="49.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="48.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="93.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="109.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="50.25" customHeight="1">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="58" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="113.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -806,461 +1309,28 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="45">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="76.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="71.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="49.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="49.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="40.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="48.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="93.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="109.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="30">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="50.25" customHeight="1">
-      <c r="A1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="58" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="38.28515625" customWidth="1"/>
-    <col min="2" max="2" width="59.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="45">
-      <c r="A2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="38.28515625" customWidth="1"/>
-    <col min="2" max="2" width="59.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="45">
-      <c r="A2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>